<commit_message>
comparations of vertica and beo4j
</commit_message>
<xml_diff>
--- a/exp/数据量-vertica.xlsx
+++ b/exp/数据量-vertica.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBC16E6-AD3B-4526-9603-F9DDA566720F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8549D37D-B2B1-4F22-9160-71F2A10044F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>1GB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,6 +33,14 @@
     <t>100GB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Vertica</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neo4j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -41,7 +49,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +62,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -77,9 +92,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -266,7 +287,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$3</c:f>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -283,7 +304,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$3</c:f>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="3"/>
@@ -396,7 +417,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$2</c:f>
+              <c:f>Sheet1!$C$2:$C$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -458,7 +479,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="zh-CN" altLang="en-US"/>
-                  <a:t>数据大小</a:t>
+                  <a:t>数据量</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -602,6 +623,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.39686752697579458"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -666,6 +695,45 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -749,7 +817,1162 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vertica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1GB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10GB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.6424735427499999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0902241469500016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.934129286999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9701-4D6F-843E-A29882AE3034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neo4j</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1GB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10GB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>48.238300000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>541.86763657500001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9701-4D6F-843E-A29882AE3034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="634225528"/>
+        <c:axId val="634233400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="634225528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634233400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="634233400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634225528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Vertica-Neo4j</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>不同数据量</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>一度邻接点查询</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vertica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1GB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10GB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.33518486024999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6825459193900002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6268236565599974</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AAB-45F7-BE08-7C27760A64D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neo4j</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1GB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10GB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.90639999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.132346046249999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2AAB-45F7-BE08-7C27760A64D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="698445840"/>
+        <c:axId val="698447808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="698445840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US"/>
+                  <a:t>数据量</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698447808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="698447808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US"/>
+                  <a:t>时间</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>/s</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000_ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698445840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1292,20 +2515,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1325,6 +3554,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C77144B-D731-4157-BA38-BFA9E000FA83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>445770</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>140970</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243E0E0F-2994-47BF-ABBB-AE65772200C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1596,42 +3897,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="1">
         <v>1.6424735427499999</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>48.238300000000002</v>
       </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.33518486024999999</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.90639999999999998</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>8.0902241469500016</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>541.86763657500001</v>
       </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.6825459193900002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>10.132346046249999</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>21.934129286999998</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>9.6268236565599974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>